<commit_message>
Update RMIL data 2025-10-22 03:57:32 UTC
</commit_message>
<xml_diff>
--- a/data/RashtriyaMetal/RMIL_Price_Log.xlsx
+++ b/data/RashtriyaMetal/RMIL_Price_Log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -477,6 +477,28 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2025-10-22 03:57:32</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2025-10-20</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>https://rashtriyametal.com/wp-content/uploads/2025/10/ListPrice20102025.pdf</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>/home/runner/work/rashtriyametal_downloader/rashtriyametal_downloader/data/RashtriyaMetal/PDFs/ListPrice20102025.pdf</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update RMIL data 2025-10-24 03:49:11 UTC
</commit_message>
<xml_diff>
--- a/data/RashtriyaMetal/RMIL_Price_Log.xlsx
+++ b/data/RashtriyaMetal/RMIL_Price_Log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -499,6 +499,28 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2025-10-24 03:49:11</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2025-10-23</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>https://rashtriyametal.com/wp-content/uploads/2025/10/ListPrice23102025.pdf</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>/home/runner/work/rashtriyametal_downloader/rashtriyametal_downloader/data/RashtriyaMetal/PDFs/ListPrice23102025.pdf</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update RMIL data 2025-10-28 03:53:53 UTC
</commit_message>
<xml_diff>
--- a/data/RashtriyaMetal/RMIL_Price_Log.xlsx
+++ b/data/RashtriyaMetal/RMIL_Price_Log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -521,6 +521,28 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2025-10-28 03:53:53</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2025-10-27</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>https://rashtriyametal.com/wp-content/uploads/2025/10/ListPrice27102025.pdf</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>/home/runner/work/rashtriyametal_downloader/rashtriyametal_downloader/data/RashtriyaMetal/PDFs/ListPrice27102025.pdf</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update RMIL data 2025-11-01 03:55:45 UTC
</commit_message>
<xml_diff>
--- a/data/RashtriyaMetal/RMIL_Price_Log.xlsx
+++ b/data/RashtriyaMetal/RMIL_Price_Log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -543,6 +543,28 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2025-11-01 03:55:45</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2025-10-30</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>https://rashtriyametal.com/wp-content/uploads/2025/10/ListPrice30102025-7.pdf</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>/home/runner/work/rashtriyametal_downloader/rashtriyametal_downloader/data/RashtriyaMetal/PDFs/ListPrice30102025-7.pdf</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update RMIL data 2025-11-02 03:58:56 UTC
</commit_message>
<xml_diff>
--- a/data/RashtriyaMetal/RMIL_Price_Log.xlsx
+++ b/data/RashtriyaMetal/RMIL_Price_Log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -565,6 +565,28 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2025-11-02 03:58:56</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2025-10-30</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>https://rashtriyametal.com/wp-content/uploads/2025/11/ListPrice30102025.pdf</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>/home/runner/work/rashtriyametal_downloader/rashtriyametal_downloader/data/RashtriyaMetal/PDFs/ListPrice30102025.pdf</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update RMIL data 2025-11-11 03:57:57 UTC
</commit_message>
<xml_diff>
--- a/data/RashtriyaMetal/RMIL_Price_Log.xlsx
+++ b/data/RashtriyaMetal/RMIL_Price_Log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -587,6 +587,28 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2025-11-11 03:57:57</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>2023-03-20</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>https://rashtriyametal.com/wp-content/uploads/2023/03/HZL20032023.pdf</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>/home/runner/work/rashtriyametal_downloader/rashtriyametal_downloader/data/RashtriyaMetal/PDFs/HZL20032023.pdf</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>